<commit_message>
Update schematics and BOM
</commit_message>
<xml_diff>
--- a/HF1R00/Released/BOM/HF1R00.xlsx
+++ b/HF1R00/Released/BOM/HF1R00.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Hexabitz\Hardware\Eagle\design-automation\Modules\HF1R00\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hexabitz_Github\Hardware\HF1R0x-Hardware\HF1R00\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308AA68D-5F82-44A0-BB4F-9E2500CC80F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25AE366-FB37-4B3B-9695-027D883A324E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Qty</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>U1</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 0603</t>
   </si>
   <si>
     <t>CAP CER  10% X7R 0603</t>
@@ -233,6 +230,15 @@
   </si>
   <si>
     <t>40 Position Header Connector 0.100" (2.54mm) Through Hole Tin</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 100 Ohm 1% 0.25W(1/4W) ±100ppm/C Pad SMD Automotive T/R</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 3.9K Ohm 1% 1/10W ±100ppm/°C Molded SMD SMD Paper T/R</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 1K Ohm 1% 1/10W ±100ppm/°C Molded SMD Punched Carrier T/R</t>
   </si>
 </sst>
 </file>
@@ -670,7 +676,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -690,10 +696,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -705,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -716,23 +722,23 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -740,23 +746,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="1">
         <v>61300311121</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -764,23 +770,23 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1">
         <v>61300211121</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -788,25 +794,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -814,25 +820,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -840,25 +846,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -866,23 +872,23 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.65" x14ac:dyDescent="0.5">
@@ -890,23 +896,23 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>